<commit_message>
modifications : - changed : use tab for about page - changed : rename preview file and md file, move md jsonjs in db - changed : use md doc from db based on doc id - fixed : footer vue meta highlight on metavariable page - fixed : entity icon in title centered on mobile when no favorite - removed : readme folder attribut, icon and color
</commit_message>
<xml_diff>
--- a/data/db_source/doc.xlsx
+++ b/data/db_source/doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAD7051-3B66-A540-BEF9-9A188E9CDA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5FA82A-A4A2-EA40-91BE-3FD95963A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,18 +43,9 @@
     <t>data/pdf/pdf_wiki.pdf</t>
   </si>
   <si>
-    <t>folder_1_md</t>
-  </si>
-  <si>
     <t>md</t>
   </si>
   <si>
-    <t>example_1</t>
-  </si>
-  <si>
-    <t>data/md/folder/example_1.md</t>
-  </si>
-  <si>
     <t>pdf_online</t>
   </si>
   <si>
@@ -101,6 +92,15 @@
   </si>
   <si>
     <t>Communiqué de presse population</t>
+  </si>
+  <si>
+    <t>tourisme_exemple</t>
+  </si>
+  <si>
+    <t>Tourisme exemple</t>
+  </si>
+  <si>
+    <t>data/md/tourisme_exemple.md</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -485,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -507,16 +507,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>1716231182</v>
@@ -524,30 +524,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>1706212962</v>
@@ -555,16 +555,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>1606212962</v>
@@ -572,16 +572,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E7">
         <v>1606212963</v>
@@ -589,16 +589,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>1724323867</v>

</xml_diff>

<commit_message>
fixed : tabs_body overflow hidden without hidding the download button
</commit_message>
<xml_diff>
--- a/data/db_source/doc.xlsx
+++ b/data/db_source/doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5FA82A-A4A2-EA40-91BE-3FD95963A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DAB01A-1414-334E-B051-E76F6C948996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="500" windowWidth="21200" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <v>1706212962</v>
+        <v>1706219962</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>